<commit_message>
Obtained new results after bug fix.
</commit_message>
<xml_diff>
--- a/Device Interaction/Automation/Alarms.xlsx
+++ b/Device Interaction/Automation/Alarms.xlsx
@@ -253,7 +253,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="26">
   <si>
     <t>Application</t>
   </si>
@@ -300,7 +300,7 @@
     <t>reader</t>
   </si>
   <si>
-    <t>timeout</t>
+    <t>non-terminated</t>
   </si>
   <si>
     <t>http+json</t>
@@ -312,12 +312,15 @@
     <t>detected</t>
   </si>
   <si>
-    <t>oom</t>
-  </si>
-  <si>
     <t>no error</t>
   </si>
   <si>
+    <t>1 new conflict</t>
+  </si>
+  <si>
+    <t>1 new non conflict</t>
+  </si>
+  <si>
     <t>min</t>
   </si>
   <si>
@@ -328,12 +331,6 @@
   </si>
   <si>
     <t>Detected time:</t>
-  </si>
-  <si>
-    <t>1 new conflict</t>
-  </si>
-  <si>
-    <t>1 new non conflict</t>
   </si>
 </sst>
 </file>
@@ -406,12 +403,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF9900"/>
-        <bgColor rgb="FFFF9900"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF4A86E8"/>
         <bgColor rgb="FF4A86E8"/>
       </patternFill>
@@ -420,6 +411,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF00FFFF"/>
         <bgColor rgb="FF00FFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF9900"/>
+        <bgColor rgb="FFFF9900"/>
       </patternFill>
     </fill>
     <fill>
@@ -438,7 +435,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="54">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -467,23 +464,123 @@
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="7" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="8" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="9" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="9" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="10" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="top"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="top" wrapText="0"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="top" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0" vertical="top"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="top" wrapText="0"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="0"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="top" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="3" fontId="4" numFmtId="21" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="9" fontId="4" numFmtId="21" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="7" fontId="4" numFmtId="21" xfId="0" applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="8" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="9" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="10" fontId="4" numFmtId="21" xfId="0" applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
@@ -496,101 +593,8 @@
     <xf borderId="0" fillId="3" fontId="1" numFmtId="21" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="46" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="7" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="7" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="10" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="top"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="top" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="top" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" vertical="top"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="top" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="top" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -760,7 +764,7 @@
       <c r="D4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="E4" s="10" t="s">
         <v>18</v>
       </c>
       <c r="F4" s="9" t="s">
@@ -804,13 +808,13 @@
       <c r="D5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="E5" s="10" t="s">
         <v>18</v>
       </c>
       <c r="F5" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="11" t="s">
+      <c r="G5" s="10" t="s">
         <v>18</v>
       </c>
       <c r="H5" s="6" t="s">
@@ -858,7 +862,7 @@
         <v>15</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="I6" s="6" t="s">
         <v>13</v>
@@ -892,16 +896,16 @@
       <c r="D7" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="13" t="s">
-        <v>20</v>
+      <c r="E7" s="11" t="s">
+        <v>19</v>
       </c>
       <c r="F7" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="G7" s="14" t="s">
+      <c r="G7" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="H7" s="11" t="s">
+      <c r="H7" s="10" t="s">
         <v>18</v>
       </c>
       <c r="I7" s="9" t="s">
@@ -936,22 +940,22 @@
       <c r="D8" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="11" t="s">
+      <c r="E8" s="10" t="s">
         <v>18</v>
       </c>
       <c r="F8" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="G8" s="11" t="s">
+      <c r="G8" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="H8" s="11" t="s">
+      <c r="H8" s="10" t="s">
         <v>18</v>
       </c>
       <c r="I8" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="J8" s="11" t="s">
+      <c r="J8" s="10" t="s">
         <v>18</v>
       </c>
       <c r="K8" s="6" t="s">
@@ -987,7 +991,7 @@
         <v>15</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="H9" s="9" t="s">
         <v>15</v>
@@ -1031,7 +1035,7 @@
         <v>15</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="H10" s="9" t="s">
         <v>15</v>
@@ -1075,7 +1079,7 @@
         <v>15</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="H11" s="9" t="s">
         <v>15</v>
@@ -1100,491 +1104,452 @@
       </c>
     </row>
     <row r="12">
-      <c r="D12" s="19" t="s">
+      <c r="D12" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="E12" s="21">
+      <c r="E12" s="14">
         <f t="shared" ref="E12:N12" si="1">countif(E$2:E$11, "detected")</f>
         <v>3</v>
       </c>
-      <c r="F12" s="21">
+      <c r="F12" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G12" s="21">
+      <c r="G12" s="14">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="H12" s="21">
+      <c r="H12" s="14">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="I12" s="21">
+      <c r="I12" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J12" s="21">
+      <c r="J12" s="14">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="K12" s="21">
+      <c r="K12" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L12" s="21">
+      <c r="L12" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M12" s="21">
+      <c r="M12" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="N12" s="21">
+      <c r="N12" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O12" s="22">
-        <f t="shared" ref="O12:O15" si="3">sum(E12:N12)</f>
+      <c r="O12" s="15">
+        <f t="shared" ref="O12:O14" si="3">sum(E12:N12)</f>
         <v>9</v>
       </c>
-      <c r="P12" s="23" t="s">
-        <v>25</v>
+      <c r="P12" s="16" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="13">
-      <c r="D13" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="E13" s="21">
+      <c r="D13" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13" s="14">
         <f t="shared" ref="E13:N13" si="2">countif(E$2:E$11, "no error")</f>
         <v>1</v>
       </c>
-      <c r="F13" s="21">
+      <c r="F13" s="14">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G13" s="21">
+      <c r="G13" s="14">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H13" s="21">
+      <c r="H13" s="14">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I13" s="21">
+      <c r="I13" s="14">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J13" s="21">
+      <c r="J13" s="14">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K13" s="21">
+      <c r="K13" s="14">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="L13" s="21">
+      <c r="L13" s="14">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M13" s="21">
+      <c r="M13" s="14">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="N13" s="21">
+      <c r="N13" s="14">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O13" s="25">
+      <c r="O13" s="18">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="P13" s="26" t="s">
-        <v>26</v>
+      <c r="P13" s="19" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="14">
       <c r="D14" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="E14" s="21">
-        <f t="shared" ref="E14:N14" si="4">COUNTIF(E$3:E$11, "oom")</f>
-        <v>0</v>
-      </c>
-      <c r="F14" s="21">
+        <v>15</v>
+      </c>
+      <c r="E14" s="14">
+        <f t="shared" ref="E14:N14" si="4">COUNTIF(E$3:E$11, "non-terminated")</f>
+        <v>5</v>
+      </c>
+      <c r="F14" s="14">
+        <f t="shared" si="4"/>
+        <v>8</v>
+      </c>
+      <c r="G14" s="14">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="H14" s="14">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="I14" s="14">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+      <c r="J14" s="14">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+      <c r="K14" s="14">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+      <c r="L14" s="14">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="M14" s="14">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="N14" s="14">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="G14" s="21">
-        <f t="shared" si="4"/>
-        <v>3</v>
-      </c>
-      <c r="H14" s="21">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="I14" s="21">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="J14" s="21">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="K14" s="21">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="L14" s="21">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="M14" s="21">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="N14" s="21">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="O14" s="27">
+      <c r="O14" s="20">
         <f t="shared" si="3"/>
-        <v>4</v>
-      </c>
-      <c r="P14" s="28"/>
+        <v>35</v>
+      </c>
+      <c r="P14" s="21"/>
     </row>
     <row r="15">
-      <c r="D15" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="E15" s="21">
-        <f t="shared" ref="E15:N15" si="5">COUNTIF(E$3:E$11, "timeout")</f>
-        <v>5</v>
-      </c>
-      <c r="F15" s="21">
-        <f t="shared" si="5"/>
-        <v>8</v>
-      </c>
-      <c r="G15" s="21">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="H15" s="21">
-        <f t="shared" si="5"/>
-        <v>3</v>
-      </c>
-      <c r="I15" s="21">
-        <f t="shared" si="5"/>
-        <v>5</v>
-      </c>
-      <c r="J15" s="21">
-        <f t="shared" si="5"/>
-        <v>3</v>
-      </c>
-      <c r="K15" s="21">
-        <f t="shared" si="5"/>
-        <v>3</v>
-      </c>
-      <c r="L15" s="21">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="M15" s="21">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="N15" s="21">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="O15" s="27">
-        <f t="shared" si="3"/>
-        <v>31</v>
-      </c>
-      <c r="P15" s="28">
-        <f>sum(O14:O15)</f>
-        <v>35</v>
-      </c>
+      <c r="D15" s="1"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="14"/>
+      <c r="K15" s="14"/>
+      <c r="L15" s="14"/>
+      <c r="M15" s="14"/>
+      <c r="N15" s="14"/>
+      <c r="O15" s="22"/>
     </row>
     <row r="16">
-      <c r="D16" s="28"/>
-      <c r="E16" s="28"/>
-      <c r="F16" s="28"/>
-      <c r="G16" s="28"/>
-      <c r="H16" s="28"/>
-      <c r="I16" s="28"/>
-      <c r="J16" s="29"/>
-      <c r="K16" s="28"/>
-      <c r="L16" s="30"/>
-      <c r="M16" s="30"/>
-      <c r="N16" s="30"/>
-      <c r="O16" s="29"/>
-      <c r="P16" s="28"/>
+      <c r="D16" s="21"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="21"/>
+      <c r="G16" s="21"/>
+      <c r="H16" s="21"/>
+      <c r="I16" s="21"/>
+      <c r="J16" s="23"/>
+      <c r="K16" s="21"/>
+      <c r="L16" s="24"/>
+      <c r="M16" s="24"/>
+      <c r="N16" s="24"/>
+      <c r="O16" s="23"/>
+      <c r="P16" s="21"/>
     </row>
     <row r="17">
-      <c r="D17" s="31"/>
-      <c r="E17" s="32"/>
-      <c r="F17" s="28"/>
-      <c r="G17" s="28"/>
-      <c r="H17" s="28"/>
-      <c r="I17" s="28"/>
-      <c r="J17" s="29"/>
-      <c r="K17" s="28"/>
-      <c r="L17" s="30"/>
-      <c r="M17" s="30"/>
-      <c r="N17" s="30"/>
-      <c r="O17" s="29"/>
-      <c r="P17" s="28"/>
+      <c r="D17" s="25"/>
+      <c r="E17" s="26"/>
+      <c r="F17" s="21"/>
+      <c r="G17" s="21"/>
+      <c r="H17" s="21"/>
+      <c r="I17" s="21"/>
+      <c r="J17" s="23"/>
+      <c r="K17" s="21"/>
+      <c r="L17" s="24"/>
+      <c r="M17" s="24"/>
+      <c r="N17" s="24"/>
+      <c r="O17" s="23"/>
+      <c r="P17" s="21"/>
     </row>
     <row r="18">
-      <c r="D18" s="31"/>
-      <c r="E18" s="28"/>
-      <c r="F18" s="28"/>
-      <c r="G18" s="28"/>
-      <c r="H18" s="28"/>
-      <c r="I18" s="28"/>
-      <c r="J18" s="29"/>
-      <c r="K18" s="28"/>
-      <c r="L18" s="30"/>
-      <c r="M18" s="30"/>
-      <c r="N18" s="30"/>
-      <c r="O18" s="29"/>
-      <c r="P18" s="28"/>
+      <c r="D18" s="25"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="21"/>
+      <c r="G18" s="21"/>
+      <c r="H18" s="21"/>
+      <c r="I18" s="21"/>
+      <c r="J18" s="23"/>
+      <c r="K18" s="21"/>
+      <c r="L18" s="24"/>
+      <c r="M18" s="24"/>
+      <c r="N18" s="24"/>
+      <c r="O18" s="23"/>
+      <c r="P18" s="21"/>
     </row>
     <row r="19">
-      <c r="D19" s="28"/>
-      <c r="E19" s="28"/>
-      <c r="F19" s="28"/>
-      <c r="G19" s="28"/>
-      <c r="H19" s="28"/>
-      <c r="I19" s="28"/>
-      <c r="J19" s="29"/>
-      <c r="K19" s="28"/>
-      <c r="L19" s="30"/>
-      <c r="M19" s="30"/>
-      <c r="N19" s="30"/>
-      <c r="O19" s="29"/>
-      <c r="P19" s="28"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="21"/>
+      <c r="G19" s="21"/>
+      <c r="H19" s="21"/>
+      <c r="I19" s="21"/>
+      <c r="J19" s="23"/>
+      <c r="K19" s="21"/>
+      <c r="L19" s="24"/>
+      <c r="M19" s="24"/>
+      <c r="N19" s="24"/>
+      <c r="O19" s="23"/>
+      <c r="P19" s="21"/>
     </row>
     <row r="20">
-      <c r="D20" s="23"/>
-      <c r="E20" s="23"/>
-      <c r="F20" s="23"/>
-      <c r="G20" s="28"/>
-      <c r="H20" s="28"/>
-      <c r="I20" s="23"/>
-      <c r="J20" s="23"/>
-      <c r="K20" s="33"/>
-      <c r="L20" s="28"/>
-      <c r="M20" s="28"/>
-      <c r="N20" s="23"/>
-      <c r="O20" s="28"/>
+      <c r="D20" s="16"/>
+      <c r="E20" s="16"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="21"/>
+      <c r="H20" s="21"/>
+      <c r="I20" s="16"/>
+      <c r="J20" s="16"/>
+      <c r="K20" s="27"/>
+      <c r="L20" s="21"/>
+      <c r="M20" s="21"/>
+      <c r="N20" s="16"/>
+      <c r="O20" s="21"/>
     </row>
     <row r="21">
-      <c r="D21" s="23"/>
-      <c r="E21" s="23"/>
-      <c r="F21" s="23"/>
-      <c r="G21" s="28"/>
-      <c r="H21" s="28"/>
-      <c r="I21" s="23"/>
-      <c r="J21" s="23"/>
-      <c r="K21" s="34"/>
-      <c r="L21" s="28"/>
-      <c r="M21" s="28"/>
-      <c r="N21" s="23"/>
-      <c r="O21" s="35"/>
+      <c r="D21" s="16"/>
+      <c r="E21" s="16"/>
+      <c r="F21" s="16"/>
+      <c r="G21" s="21"/>
+      <c r="H21" s="21"/>
+      <c r="I21" s="16"/>
+      <c r="J21" s="16"/>
+      <c r="K21" s="28"/>
+      <c r="L21" s="21"/>
+      <c r="M21" s="21"/>
+      <c r="N21" s="16"/>
+      <c r="O21" s="29"/>
     </row>
     <row r="22">
-      <c r="D22" s="23"/>
-      <c r="E22" s="36"/>
-      <c r="F22" s="37"/>
-      <c r="G22" s="28"/>
-      <c r="H22" s="28"/>
-      <c r="I22" s="23"/>
-      <c r="J22" s="23"/>
-      <c r="K22" s="34"/>
-      <c r="L22" s="38"/>
-      <c r="M22" s="28"/>
-      <c r="N22" s="23"/>
-      <c r="O22" s="39"/>
+      <c r="D22" s="16"/>
+      <c r="E22" s="30"/>
+      <c r="F22" s="31"/>
+      <c r="G22" s="21"/>
+      <c r="H22" s="21"/>
+      <c r="I22" s="16"/>
+      <c r="J22" s="16"/>
+      <c r="K22" s="28"/>
+      <c r="L22" s="32"/>
+      <c r="M22" s="21"/>
+      <c r="N22" s="16"/>
+      <c r="O22" s="33"/>
     </row>
     <row r="23">
-      <c r="D23" s="23"/>
-      <c r="E23" s="36"/>
-      <c r="F23" s="37"/>
-      <c r="G23" s="28"/>
-      <c r="H23" s="28"/>
-      <c r="I23" s="23"/>
-      <c r="J23" s="23"/>
-      <c r="K23" s="40"/>
-      <c r="L23" s="38"/>
-      <c r="M23" s="38"/>
-      <c r="N23" s="23"/>
-      <c r="O23" s="35"/>
+      <c r="D23" s="16"/>
+      <c r="E23" s="30"/>
+      <c r="F23" s="31"/>
+      <c r="G23" s="21"/>
+      <c r="H23" s="21"/>
+      <c r="I23" s="16"/>
+      <c r="J23" s="16"/>
+      <c r="K23" s="34"/>
+      <c r="L23" s="32"/>
+      <c r="M23" s="32"/>
+      <c r="N23" s="16"/>
+      <c r="O23" s="29"/>
     </row>
     <row r="24">
-      <c r="D24" s="23"/>
-      <c r="E24" s="26"/>
-      <c r="F24" s="41"/>
-      <c r="G24" s="28"/>
-      <c r="H24" s="28"/>
-      <c r="I24" s="23"/>
-      <c r="J24" s="23"/>
-      <c r="K24" s="42"/>
-      <c r="L24" s="28"/>
-      <c r="M24" s="28"/>
-      <c r="N24" s="23"/>
-      <c r="O24" s="35"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="19"/>
+      <c r="F24" s="35"/>
+      <c r="G24" s="21"/>
+      <c r="H24" s="21"/>
+      <c r="I24" s="16"/>
+      <c r="J24" s="16"/>
+      <c r="K24" s="36"/>
+      <c r="L24" s="21"/>
+      <c r="M24" s="21"/>
+      <c r="N24" s="16"/>
+      <c r="O24" s="29"/>
     </row>
     <row r="25">
-      <c r="D25" s="23"/>
-      <c r="E25" s="26"/>
-      <c r="F25" s="26"/>
-      <c r="G25" s="38"/>
-      <c r="H25" s="28"/>
-      <c r="I25" s="23"/>
-      <c r="J25" s="23"/>
-      <c r="K25" s="40"/>
-      <c r="L25" s="38"/>
-      <c r="M25" s="28"/>
-      <c r="N25" s="23"/>
-      <c r="O25" s="35"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="19"/>
+      <c r="F25" s="19"/>
+      <c r="G25" s="32"/>
+      <c r="H25" s="21"/>
+      <c r="I25" s="16"/>
+      <c r="J25" s="16"/>
+      <c r="K25" s="34"/>
+      <c r="L25" s="32"/>
+      <c r="M25" s="21"/>
+      <c r="N25" s="16"/>
+      <c r="O25" s="29"/>
     </row>
     <row r="26">
-      <c r="D26" s="23"/>
-      <c r="E26" s="26"/>
-      <c r="F26" s="26"/>
-      <c r="G26" s="38"/>
-      <c r="H26" s="28"/>
-      <c r="I26" s="23"/>
-      <c r="J26" s="23"/>
-      <c r="K26" s="23"/>
-      <c r="L26" s="23"/>
-      <c r="M26" s="23"/>
-      <c r="N26" s="23"/>
-      <c r="O26" s="23"/>
+      <c r="D26" s="16"/>
+      <c r="E26" s="19"/>
+      <c r="F26" s="19"/>
+      <c r="G26" s="32"/>
+      <c r="H26" s="21"/>
+      <c r="I26" s="16"/>
+      <c r="J26" s="16"/>
+      <c r="K26" s="16"/>
+      <c r="L26" s="16"/>
+      <c r="M26" s="16"/>
+      <c r="N26" s="16"/>
+      <c r="O26" s="16"/>
     </row>
     <row r="27">
-      <c r="D27" s="23"/>
-      <c r="E27" s="43"/>
-      <c r="F27" s="43"/>
-      <c r="G27" s="38"/>
-      <c r="H27" s="28"/>
-      <c r="I27" s="23"/>
-      <c r="J27" s="23"/>
-      <c r="K27" s="33"/>
-      <c r="L27" s="28"/>
-      <c r="M27" s="28"/>
-      <c r="N27" s="23"/>
-      <c r="O27" s="28"/>
+      <c r="D27" s="16"/>
+      <c r="E27" s="37"/>
+      <c r="F27" s="37"/>
+      <c r="G27" s="32"/>
+      <c r="H27" s="21"/>
+      <c r="I27" s="16"/>
+      <c r="J27" s="16"/>
+      <c r="K27" s="27"/>
+      <c r="L27" s="21"/>
+      <c r="M27" s="21"/>
+      <c r="N27" s="16"/>
+      <c r="O27" s="21"/>
     </row>
     <row r="28">
-      <c r="D28" s="23"/>
-      <c r="E28" s="23"/>
-      <c r="F28" s="23"/>
-      <c r="G28" s="28"/>
-      <c r="H28" s="28"/>
-      <c r="I28" s="23"/>
-      <c r="J28" s="23"/>
-      <c r="K28" s="44"/>
-      <c r="L28" s="38"/>
-      <c r="M28" s="38"/>
-      <c r="N28" s="23"/>
-      <c r="O28" s="39"/>
+      <c r="D28" s="16"/>
+      <c r="E28" s="16"/>
+      <c r="F28" s="16"/>
+      <c r="G28" s="21"/>
+      <c r="H28" s="21"/>
+      <c r="I28" s="16"/>
+      <c r="J28" s="16"/>
+      <c r="K28" s="38"/>
+      <c r="L28" s="32"/>
+      <c r="M28" s="32"/>
+      <c r="N28" s="16"/>
+      <c r="O28" s="33"/>
     </row>
     <row r="29">
-      <c r="D29" s="23"/>
-      <c r="E29" s="23"/>
-      <c r="F29" s="23"/>
-      <c r="G29" s="28"/>
-      <c r="H29" s="28"/>
-      <c r="I29" s="23"/>
-      <c r="J29" s="23"/>
-      <c r="K29" s="45"/>
-      <c r="L29" s="38"/>
-      <c r="M29" s="38"/>
-      <c r="N29" s="23"/>
-      <c r="O29" s="39"/>
+      <c r="D29" s="16"/>
+      <c r="E29" s="16"/>
+      <c r="F29" s="16"/>
+      <c r="G29" s="21"/>
+      <c r="H29" s="21"/>
+      <c r="I29" s="16"/>
+      <c r="J29" s="16"/>
+      <c r="K29" s="39"/>
+      <c r="L29" s="32"/>
+      <c r="M29" s="32"/>
+      <c r="N29" s="16"/>
+      <c r="O29" s="33"/>
     </row>
     <row r="30">
-      <c r="D30" s="23"/>
-      <c r="E30" s="23"/>
-      <c r="F30" s="23"/>
-      <c r="G30" s="28"/>
-      <c r="H30" s="28"/>
-      <c r="I30" s="23"/>
-      <c r="J30" s="23"/>
-      <c r="K30" s="46"/>
-      <c r="L30" s="28"/>
-      <c r="M30" s="28"/>
-      <c r="N30" s="23"/>
-      <c r="O30" s="35"/>
+      <c r="D30" s="16"/>
+      <c r="E30" s="16"/>
+      <c r="F30" s="16"/>
+      <c r="G30" s="21"/>
+      <c r="H30" s="21"/>
+      <c r="I30" s="16"/>
+      <c r="J30" s="16"/>
+      <c r="K30" s="40"/>
+      <c r="L30" s="21"/>
+      <c r="M30" s="21"/>
+      <c r="N30" s="16"/>
+      <c r="O30" s="29"/>
     </row>
     <row r="31">
-      <c r="D31" s="23"/>
-      <c r="E31" s="23"/>
-      <c r="F31" s="23"/>
-      <c r="G31" s="28"/>
-      <c r="H31" s="28"/>
-      <c r="I31" s="23"/>
-      <c r="J31" s="23"/>
-      <c r="K31" s="47"/>
-      <c r="L31" s="28"/>
-      <c r="M31" s="28"/>
-      <c r="N31" s="23"/>
-      <c r="O31" s="35"/>
+      <c r="D31" s="16"/>
+      <c r="E31" s="16"/>
+      <c r="F31" s="16"/>
+      <c r="G31" s="21"/>
+      <c r="H31" s="21"/>
+      <c r="I31" s="16"/>
+      <c r="J31" s="16"/>
+      <c r="K31" s="41"/>
+      <c r="L31" s="21"/>
+      <c r="M31" s="21"/>
+      <c r="N31" s="16"/>
+      <c r="O31" s="29"/>
     </row>
     <row r="32">
-      <c r="D32" s="23"/>
-      <c r="E32" s="23"/>
-      <c r="F32" s="23"/>
-      <c r="G32" s="28"/>
-      <c r="H32" s="28"/>
-      <c r="I32" s="23"/>
-      <c r="J32" s="23"/>
-      <c r="K32" s="48"/>
-      <c r="L32" s="28"/>
-      <c r="M32" s="28"/>
-      <c r="N32" s="23"/>
-      <c r="O32" s="32"/>
+      <c r="D32" s="16"/>
+      <c r="E32" s="16"/>
+      <c r="F32" s="16"/>
+      <c r="G32" s="21"/>
+      <c r="H32" s="21"/>
+      <c r="I32" s="16"/>
+      <c r="J32" s="16"/>
+      <c r="K32" s="42"/>
+      <c r="L32" s="21"/>
+      <c r="M32" s="21"/>
+      <c r="N32" s="16"/>
+      <c r="O32" s="26"/>
     </row>
     <row r="33">
-      <c r="D33" s="23"/>
-      <c r="E33" s="23"/>
-      <c r="F33" s="23"/>
-      <c r="G33" s="23"/>
-      <c r="H33" s="23"/>
-      <c r="I33" s="23"/>
-      <c r="J33" s="23"/>
-      <c r="K33" s="33"/>
-      <c r="L33" s="28"/>
-      <c r="M33" s="28"/>
-      <c r="N33" s="23"/>
-      <c r="O33" s="39"/>
+      <c r="D33" s="16"/>
+      <c r="E33" s="16"/>
+      <c r="F33" s="16"/>
+      <c r="G33" s="16"/>
+      <c r="H33" s="16"/>
+      <c r="I33" s="16"/>
+      <c r="J33" s="16"/>
+      <c r="K33" s="27"/>
+      <c r="L33" s="21"/>
+      <c r="M33" s="21"/>
+      <c r="N33" s="16"/>
+      <c r="O33" s="33"/>
     </row>
     <row r="38">
       <c r="E38" s="1"/>
-      <c r="G38" s="49"/>
+      <c r="G38" s="43"/>
     </row>
     <row r="39">
       <c r="E39" s="1"/>
-      <c r="G39" s="49"/>
+      <c r="G39" s="43"/>
     </row>
     <row r="40">
       <c r="E40" s="1"/>
-      <c r="G40" s="50"/>
+      <c r="G40" s="44"/>
     </row>
     <row r="41">
       <c r="E41" s="1"/>
-      <c r="G41" s="50"/>
+      <c r="G41" s="44"/>
     </row>
     <row r="42">
       <c r="E42" s="1"/>
-      <c r="G42" s="49"/>
+      <c r="G42" s="43"/>
     </row>
     <row r="43">
       <c r="E43" s="1"/>
-      <c r="G43" s="49"/>
+      <c r="G43" s="43"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -1705,7 +1670,7 @@
       <c r="D3" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="9"/>
+      <c r="E3" s="45"/>
       <c r="F3" s="6" t="s">
         <v>13</v>
       </c>
@@ -1747,10 +1712,10 @@
       <c r="D4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="10">
-        <v>5.902777777777778E-4</v>
-      </c>
-      <c r="F4" s="9"/>
+      <c r="E4" s="46">
+        <v>9.259259259259259E-5</v>
+      </c>
+      <c r="F4" s="45"/>
       <c r="G4" s="6" t="s">
         <v>13</v>
       </c>
@@ -1789,11 +1754,11 @@
       <c r="D5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="10">
-        <v>5.092592592592592E-4</v>
-      </c>
-      <c r="F5" s="9"/>
-      <c r="G5" s="10">
+      <c r="E5" s="46">
+        <v>6.944444444444444E-5</v>
+      </c>
+      <c r="F5" s="45"/>
+      <c r="G5" s="46">
         <v>0.0012037037037037038</v>
       </c>
       <c r="H5" s="6" t="s">
@@ -1831,10 +1796,10 @@
       <c r="D6" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
+      <c r="E6" s="45"/>
+      <c r="F6" s="45"/>
+      <c r="G6" s="45"/>
+      <c r="H6" s="45"/>
       <c r="I6" s="6" t="s">
         <v>13</v>
       </c>
@@ -1867,15 +1832,15 @@
       <c r="D7" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="12"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="10">
-        <v>4.5138888888888887E-4</v>
-      </c>
-      <c r="H7" s="10">
-        <v>4.976851851851852E-4</v>
-      </c>
-      <c r="I7" s="9"/>
+      <c r="E7" s="47"/>
+      <c r="F7" s="45"/>
+      <c r="G7" s="46">
+        <v>9.259259259259259E-5</v>
+      </c>
+      <c r="H7" s="46">
+        <v>6.944444444444444E-5</v>
+      </c>
+      <c r="I7" s="45"/>
       <c r="J7" s="6" t="s">
         <v>13</v>
       </c>
@@ -1905,19 +1870,19 @@
       <c r="D8" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="10">
-        <v>7.754629629629629E-4</v>
-      </c>
-      <c r="F8" s="9"/>
-      <c r="G8" s="10">
-        <v>6.597222222222222E-4</v>
-      </c>
-      <c r="H8" s="10">
-        <v>9.606481481481482E-4</v>
-      </c>
-      <c r="I8" s="9"/>
-      <c r="J8" s="10">
-        <v>6.481481481481481E-4</v>
+      <c r="E8" s="46">
+        <v>5.555555555555556E-4</v>
+      </c>
+      <c r="F8" s="45"/>
+      <c r="G8" s="46">
+        <v>0.0012152777777777778</v>
+      </c>
+      <c r="H8" s="46">
+        <v>1.7361111111111112E-4</v>
+      </c>
+      <c r="I8" s="45"/>
+      <c r="J8" s="46">
+        <v>7.638888888888889E-4</v>
       </c>
       <c r="K8" s="6" t="s">
         <v>13</v>
@@ -1945,13 +1910,13 @@
       <c r="D9" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
-      <c r="J9" s="9"/>
-      <c r="K9" s="9"/>
+      <c r="E9" s="45"/>
+      <c r="F9" s="45"/>
+      <c r="G9" s="45"/>
+      <c r="H9" s="45"/>
+      <c r="I9" s="45"/>
+      <c r="J9" s="45"/>
+      <c r="K9" s="45"/>
       <c r="L9" s="6" t="s">
         <v>13</v>
       </c>
@@ -1975,14 +1940,14 @@
       <c r="D10" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9"/>
-      <c r="K10" s="9"/>
-      <c r="L10" s="9"/>
+      <c r="E10" s="45"/>
+      <c r="F10" s="45"/>
+      <c r="G10" s="45"/>
+      <c r="H10" s="45"/>
+      <c r="I10" s="45"/>
+      <c r="J10" s="45"/>
+      <c r="K10" s="45"/>
+      <c r="L10" s="45"/>
       <c r="M10" s="6" t="s">
         <v>13</v>
       </c>
@@ -2003,47 +1968,50 @@
       <c r="D11" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9"/>
-      <c r="J11" s="9"/>
-      <c r="K11" s="9"/>
-      <c r="L11" s="9"/>
-      <c r="M11" s="9"/>
+      <c r="E11" s="45"/>
+      <c r="F11" s="45"/>
+      <c r="G11" s="45"/>
+      <c r="H11" s="45"/>
+      <c r="I11" s="45"/>
+      <c r="J11" s="45"/>
+      <c r="K11" s="45"/>
+      <c r="L11" s="45"/>
+      <c r="M11" s="45"/>
       <c r="N11" s="6" t="s">
         <v>13</v>
       </c>
     </row>
+    <row r="12">
+      <c r="D12" s="48"/>
+    </row>
     <row r="13">
-      <c r="D13" s="15"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="G13" s="17" t="s">
+      <c r="D13" s="49"/>
+      <c r="E13" s="50"/>
+      <c r="F13" s="51" t="s">
         <v>22</v>
       </c>
-      <c r="H13" s="17" t="s">
+      <c r="G13" s="51" t="s">
         <v>23</v>
       </c>
+      <c r="H13" s="51" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="14">
-      <c r="E14" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="F14" s="20">
+      <c r="E14" s="52" t="s">
+        <v>25</v>
+      </c>
+      <c r="F14" s="53">
         <f>MIN(E2:N11)</f>
-        <v>0.0004513888889</v>
-      </c>
-      <c r="G14" s="20">
+        <v>0.00006944444444</v>
+      </c>
+      <c r="G14" s="53">
         <f>MAX(E2:N11)</f>
-        <v>0.001203703704</v>
-      </c>
-      <c r="H14" s="20">
+        <v>0.001215277778</v>
+      </c>
+      <c r="H14" s="53">
         <f>AVERAGE(E2:N11)</f>
-        <v>0.0006995884774</v>
+        <v>0.0004706790123</v>
       </c>
     </row>
   </sheetData>

</xml_diff>